<commit_message>
Add a datatable and model to add users for System Admin
</commit_message>
<xml_diff>
--- a/Documents/Use_Case/UserFunctions-Final-Inventory.xlsx
+++ b/Documents/Use_Case/UserFunctions-Final-Inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SALINDA SANDARUWAN\SIBA_Dynamics\Inventory_System\Use_Case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SALINDA SANDARUWAN\SIBA_Dynamics\SIBA-Inventory-system-Dynamics\Inventory-2k23\Documents\Use_Case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F81307-1F16-4BDE-BB28-0B690379AFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C900FF4B-DC81-4465-B3DB-3398304C6E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,12 +75,6 @@
 Select multiple items and send a list.</t>
   </si>
   <si>
-    <t>DepartmentUser</t>
-  </si>
-  <si>
-    <t>DepartmentAdminUser</t>
-  </si>
-  <si>
     <t>StoreManager</t>
   </si>
   <si>
@@ -286,6 +280,12 @@
   </si>
   <si>
     <t xml:space="preserve">Create Order new items </t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>DepartmentHead</t>
   </si>
 </sst>
 </file>
@@ -805,8 +805,8 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6E3506BB-5185-43B8-A011-BD6224530138}" name="Functions" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{297A1257-CBF7-43C7-8848-844759A8AF9D}" name="Note" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{66355B06-B03B-4770-9233-04AD14FCE8EB}" name="DepartmentUser" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1E888BCB-CC02-47A3-BEB0-1D8AEC24558F}" name="DepartmentAdminUser" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{66355B06-B03B-4770-9233-04AD14FCE8EB}" name="User" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1E888BCB-CC02-47A3-BEB0-1D8AEC24558F}" name="DepartmentHead" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{8EF4C5E1-0A19-4CB2-AA4F-2F1ECCE8AA99}" name="StoreManager" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{429BDD78-CD2E-4B1B-B7EF-B86AC36F0526}" name="PurchasingManager" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{B24250E2-8BDE-48C8-B483-9DDA4710E91A}" name="HeadofAdministration" dataDxfId="1"/>
@@ -1082,7 +1082,7 @@
   <dimension ref="A2:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,16 +1102,16 @@
   <sheetData>
     <row r="2" spans="3:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D2" s="42" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E2" s="41"/>
     </row>
     <row r="3" spans="3:11" ht="21" x14ac:dyDescent="0.3">
       <c r="D3" s="43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.3">
@@ -1122,22 +1122,22 @@
         <v>6</v>
       </c>
       <c r="F5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="K5" s="23" t="s">
         <v>13</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.3">
@@ -1195,10 +1195,10 @@
     <row r="10" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C10" s="22"/>
       <c r="D10" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
@@ -1206,7 +1206,7 @@
       <c r="I10" s="20"/>
       <c r="J10" s="20"/>
       <c r="K10" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.3">
@@ -1222,10 +1222,10 @@
     <row r="12" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C12" s="22"/>
       <c r="D12" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
@@ -1245,10 +1245,10 @@
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I13" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J13" s="27"/>
       <c r="K13" s="24"/>
@@ -1256,14 +1256,14 @@
     <row r="14" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C14" s="22"/>
       <c r="D14" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" s="27"/>
       <c r="G14" s="28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -1273,10 +1273,10 @@
     <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C15" s="22"/>
       <c r="D15" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F15" s="27"/>
       <c r="G15" s="28"/>
@@ -1288,14 +1288,14 @@
     <row r="16" spans="3:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="C16" s="22"/>
       <c r="D16" s="35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="36" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="37"/>
       <c r="G16" s="36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H16" s="38"/>
       <c r="I16" s="37"/>
@@ -1305,17 +1305,17 @@
     <row r="17" spans="3:12" ht="72" x14ac:dyDescent="0.3">
       <c r="C17" s="22"/>
       <c r="D17" s="35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E17" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H17" s="36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I17" s="37"/>
       <c r="J17" s="37"/>
@@ -1323,29 +1323,29 @@
     </row>
     <row r="18" spans="3:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="D18" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I18" s="28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J18" s="27"/>
       <c r="K18" s="21"/>
     </row>
     <row r="19" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D19" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="33"/>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="20" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D20" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="20"/>
@@ -1369,10 +1369,10 @@
     </row>
     <row r="21" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D21" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
@@ -1383,12 +1383,12 @@
     </row>
     <row r="22" spans="3:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="D22" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="27"/>
       <c r="G22" s="29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H22" s="29"/>
       <c r="I22" s="27"/>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="23" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D23" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="20"/>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="24" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="20"/>
@@ -1431,10 +1431,10 @@
     </row>
     <row r="26" spans="3:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D26" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="27"/>
@@ -1445,7 +1445,7 @@
     </row>
     <row r="27" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D27" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="20"/>
@@ -1458,7 +1458,7 @@
     </row>
     <row r="28" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D28" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="20"/>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="30" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D30" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="20"/>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="31" spans="3:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D31" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="20"/>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="32" spans="3:12" x14ac:dyDescent="0.3">
       <c r="D32" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="20"/>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D34" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="20"/>
@@ -1541,7 +1541,7 @@
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D35" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="20"/>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D36" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="20"/>
@@ -1565,7 +1565,7 @@
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D37" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="20"/>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D39" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="20"/>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D40" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="20"/>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D41" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="20"/>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D43" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="20"/>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D44" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="20"/>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D45" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="20"/>
@@ -1684,7 +1684,7 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="21"/>
@@ -1696,7 +1696,7 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="21"/>
@@ -1707,13 +1707,13 @@
       <c r="F49" s="20"/>
       <c r="G49" s="20"/>
       <c r="H49" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I49" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J49" s="34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K49" s="20"/>
     </row>
@@ -1722,13 +1722,13 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E53"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E54"/>
     </row>
@@ -1737,26 +1737,26 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>

</xml_diff>